<commit_message>
persist debugScript setting fixed settings not refreshed bug added tests with python and perl fixed bug with stdout/stderr at process end
</commit_message>
<xml_diff>
--- a/test/testScriptAddin.xlsx
+++ b/test/testScriptAddin.xlsx
@@ -8,31 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ScriptAddin\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C0841-8CB8-46E3-89FE-0A9BA17DCBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F2ADE3-ECB3-4AA8-BE91-06470DDBEE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="195" windowWidth="23790" windowHeight="14925" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
     <sheet name="Test_scriptRng" sheetId="7" r:id="rId2"/>
     <sheet name="Test_OtherSheet" sheetId="5" r:id="rId3"/>
+    <sheet name="Test_python" sheetId="8" r:id="rId4"/>
+    <sheet name="Test_perl" sheetId="9" r:id="rId5"/>
+    <sheet name="Test_cscript" sheetId="10" r:id="rId6"/>
+    <sheet name="Test_cmdshell" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="Data" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_1" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_10" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_11" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_12" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_13" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_14" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_2" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_3" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_4" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_5" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_6" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_7" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_8" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_9" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="Script_" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
     <definedName name="Script_">'Main Test'!$J$1:$L$5</definedName>
     <definedName name="Script_AnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
@@ -41,6 +30,8 @@
     <definedName name="Script_NewResDiagDir">'Main Test'!$S$1:$U$5</definedName>
     <definedName name="Script_ScriptCell" localSheetId="1">Test_scriptRng!$A$21:$C$25</definedName>
     <definedName name="Script_ScriptRange" localSheetId="1">Test_scriptRng!$A$15:$C$19</definedName>
+    <definedName name="Script_TestPerlCell">Test_perl!$A$1:$C$5</definedName>
+    <definedName name="Script_TestPythonCell">Test_python!$A$1:$C$5</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$13</definedName>
     <definedName name="test_in" localSheetId="2">Test_OtherSheet!$B$1:$H$4</definedName>
     <definedName name="test_in">'Main Test'!$B$1:$H$301</definedName>
@@ -49,6 +40,8 @@
     <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$17</definedName>
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
+    <definedName name="testdiagramperl">Test_perl!$E$1</definedName>
+    <definedName name="testdiagrampython">Test_python!$D$1</definedName>
     <definedName name="variablesVerzeichnis">'Main Test'!$U$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -156,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="50">
   <si>
     <t/>
   </si>
@@ -311,6 +304,61 @@
 print("Press Enter to continue...")
 invisible(scan("stdin", character(), nlines = 1, quiet = TRUE))</t>
   </si>
+  <si>
+    <t>testdiagrampython</t>
+  </si>
+  <si>
+    <t>testdiagramperl</t>
+  </si>
+  <si>
+    <t>import matplotlib.pyplot as plt
+import numpy as np
+from inspect import getsourcefile
+from os.path import abspath, dirname
+from os import chdir
+print("changing to script dir..")
+scriptpath = dirname(abspath(getsourcefile(lambda:0)))
+chdir(scriptpath)
+print("loading data ..")
+csvfile = np.loadtxt('test_in.txt',skiprows=1,unpack=True)
+np.savetxt('test_out.txt',csvfile[1])
+print(csvfile[1],csvfile[2])
+print("plotting data ..")
+plt.scatter(csvfile[1],csvfile[2])
+plt.ylabel('in2')
+plt.xlabel('in1')
+plt.savefig("testdiagrampython.png", dpi=300, format='png')
+print("finished ..")</t>
+  </si>
+  <si>
+    <t>use GD::Graph::points;
+open(SRC, '&lt;test_in.txt') or die $!;
+my (@in1, @in2);
+while (&lt;SRC&gt;) {
+    chomp;
+    my @line = split /\t/;
+    next if $line[1] eq "in2";
+    print $line[1]." ... ".$line[2]."\n";
+    push @in1, $line[1];
+    push @in2, $line[2];
+}
+close SRC;
+open(TGT, '&gt;test_out.txt') or die $!;
+print TGT $_."\n" for @in2;
+close TGT;
+print "plotting data\n";
+my @data = ([@in1], [@in2]);
+my $graph = GD::Graph::points-&gt;new(500, 300);
+$graph-&gt;set(
+                        x_label     =&gt; 'in1',
+                        y_label     =&gt; 'in2',
+                    ) or warn $mygraph-&gt;error;
+my $gd = $graph-&gt;plot(\@data) or die $graph-&gt;error;
+open(IMG, '&gt;testdiagramperl.png') or die $!;
+binmode IMG;
+print IMG $gd-&gt;png;
+print "finished \n";</t>
+  </si>
 </sst>
 </file>
 
@@ -371,74 +419,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -450,7 +436,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -465,20 +451,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -593,16 +578,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1333500</xdr:rowOff>
+      <xdr:rowOff>1362075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -631,7 +616,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7572375" y="161925"/>
+          <a:off x="7896225" y="190500"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -688,6 +673,116 @@
         <a:xfrm>
           <a:off x="2609850" y="2590800"/>
           <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518172</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>17154</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="testdiagrampython.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CFE719-8492-4496-8EE8-9F51816420E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="0"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>189905</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2695218</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="testdiagramperl.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CDF1B4-27D8-477F-91C5-B70B85A475B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648450" y="0"/>
+          <a:ext cx="4761905" cy="2857143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1024,7 +1119,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O5"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1090,7 +1185,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1147,7 +1242,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
-        <v>0.30690000000000001</v>
+        <v>0.81410000000000005</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1204,7 +1299,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
-        <v>1.04E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1260,12 +1355,12 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
-        <v>5.1000000000000004E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1321,12 +1416,12 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
-        <v>0.21249999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1356,7 +1451,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
-        <v>5.4999999999999997E-3</v>
+        <v>1.44E-2</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1383,14 +1478,14 @@
       <c r="J7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="U7" s="20" t="str">
+      <c r="U7" s="13" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1420,7 +1515,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1450,7 +1545,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
-        <v>2.3E-2</v>
+        <v>5.4100000000000002E-2</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1480,7 +1575,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
-        <v>0.3836</v>
+        <v>1.0176000000000001</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1510,7 +1605,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
-        <v>0.34520000000000001</v>
+        <v>0.91579999999999995</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1540,7 +1635,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1570,7 +1665,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1600,7 +1695,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
-        <v>1.0200000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1630,7 +1725,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1660,7 +1755,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1690,7 +1785,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1720,7 +1815,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1750,7 +1845,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1780,7 +1875,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1810,7 +1905,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>1.9099999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -1840,7 +1935,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
-        <v>4.2500000000000003E-2</v>
+        <v>0.1</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -1870,7 +1965,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>3.8300000000000001E-2</v>
+        <v>9.01E-2</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -1900,7 +1995,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
-        <v>0.44500000000000001</v>
+        <v>1.1803999999999999</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -1930,7 +2025,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
-        <v>0.32979999999999998</v>
+        <v>0.875</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -1960,7 +2055,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
-        <v>0.36049999999999999</v>
+        <v>0.95640000000000003</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -1990,7 +2085,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
-        <v>0.1918</v>
+        <v>0.50880000000000003</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -2020,7 +2115,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>1.84E-2</v>
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2050,7 +2145,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
-        <v>1.26E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2080,7 +2175,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>1.26E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2110,7 +2205,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2140,7 +2235,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>0.34</v>
+        <v>0.8</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2168,7 +2263,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
-        <v>0.255</v>
+        <v>0.6</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2195,7 +2290,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
-        <v>0.255</v>
+        <v>0.6</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2222,7 +2317,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>0.2</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2249,7 +2344,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
-        <v>1.15E-2</v>
+        <v>3.0499999999999999E-2</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2276,7 +2371,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
-        <v>6.6E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2303,7 +2398,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
-        <v>6.6E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2330,7 +2425,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
-        <v>2.7000000000000001E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2357,7 +2452,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2384,7 +2479,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2411,7 +2506,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
-        <v>1.49E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2438,7 +2533,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2465,7 +2560,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
-        <v>5.9499999999999997E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2492,7 +2587,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2519,7 +2614,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
-        <v>3.61E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2546,7 +2641,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2571,10 +2666,13 @@
       </c>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
+        <v>0.04</v>
+      </c>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I50" s="7"/>
     </row>
   </sheetData>
@@ -2592,8 +2690,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2686,7 +2784,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210710/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210728/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2720,7 +2818,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20210710/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20210728/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2812,7 +2910,7 @@
       </c>
       <c r="C18" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -2829,7 +2927,7 @@
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -2848,10 +2946,10 @@
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C21"/>
@@ -2862,10 +2960,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C22"/>
@@ -2875,24 +2973,24 @@
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C23"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="14"/>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C24"/>
@@ -2903,7 +3001,7 @@
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -2918,7 +3016,7 @@
     </row>
     <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26"/>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C26"/>
@@ -9070,7 +9168,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="12">
         <v>0.5</v>
       </c>
       <c r="D2">
@@ -9103,7 +9201,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="12">
         <v>0.6</v>
       </c>
       <c r="D3">
@@ -9137,7 +9235,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="12">
         <v>0.8</v>
       </c>
       <c r="D4">
@@ -9187,7 +9285,7 @@
         <v>40</v>
       </c>
       <c r="O7" s="4"/>
-      <c r="P7" s="23"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8"/>
@@ -9359,4 +9457,149 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E53A6E-2604-4578-8654-8C7F2E62C0EC}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65D33DA-8813-4379-A28B-0EF367670337}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="344.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D836FE-DB83-4BD9-ADBD-5E2BC66117E2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CF1B26-A656-4BDC-B33A-EB9111C2BAE8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
persist debugScript setting fixed settings not refreshed bug added tests with python, perl, jscript and cmdshell fixed bug with stdout/stderr at process end
</commit_message>
<xml_diff>
--- a/test/testScriptAddin.xlsx
+++ b/test/testScriptAddin.xlsx
@@ -8,31 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ScriptAddin\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C0841-8CB8-46E3-89FE-0A9BA17DCBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB98C77-AA4F-4998-BC95-F8691647DA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="765" windowWidth="23790" windowHeight="14925" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
     <sheet name="Test_scriptRng" sheetId="7" r:id="rId2"/>
     <sheet name="Test_OtherSheet" sheetId="5" r:id="rId3"/>
+    <sheet name="Test_python" sheetId="8" r:id="rId4"/>
+    <sheet name="Test_perl" sheetId="9" r:id="rId5"/>
+    <sheet name="Test_cscript" sheetId="10" r:id="rId6"/>
+    <sheet name="Test_cmdshell" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="Data" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_1" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_10" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_11" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_12" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_13" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_14" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_2" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_3" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_4" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_5" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_6" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_7" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_8" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
-    <definedName name="Data_9" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data" localSheetId="2">Test_OtherSheet!$A$2:$A$48</definedName>
     <definedName name="Script_" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
     <definedName name="Script_">'Main Test'!$J$1:$L$5</definedName>
     <definedName name="Script_AnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
@@ -41,6 +31,10 @@
     <definedName name="Script_NewResDiagDir">'Main Test'!$S$1:$U$5</definedName>
     <definedName name="Script_ScriptCell" localSheetId="1">Test_scriptRng!$A$21:$C$25</definedName>
     <definedName name="Script_ScriptRange" localSheetId="1">Test_scriptRng!$A$15:$C$19</definedName>
+    <definedName name="Script_TestCmdShell">Test_cmdshell!$A$1:$C$4</definedName>
+    <definedName name="Script_TestJscriptCell">Test_cscript!$A$1:$C$4</definedName>
+    <definedName name="Script_TestPerlCell">Test_perl!$A$1:$C$5</definedName>
+    <definedName name="Script_TestPythonCell">Test_python!$A$1:$C$5</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$13</definedName>
     <definedName name="test_in" localSheetId="2">Test_OtherSheet!$B$1:$H$4</definedName>
     <definedName name="test_in">'Main Test'!$B$1:$H$301</definedName>
@@ -49,6 +43,8 @@
     <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$17</definedName>
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
+    <definedName name="testdiagramperl">Test_perl!$E$1</definedName>
+    <definedName name="testdiagrampython">Test_python!$D$1</definedName>
     <definedName name="variablesVerzeichnis">'Main Test'!$U$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -89,63 +85,70 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="test_out2" type="6" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{410C0FA3-7542-41AB-90A9-C19D5D697CAD}" name="test_out11" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr prompt="0" sourceFile="C:\dev\ScriptAddin\test\.\test_out.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="test_out2" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="test_out21" type="6" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="test_out21" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out2.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="test_out3" type="6" refreshedVersion="0" background="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="test_out3" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="test_out4" type="6" refreshedVersion="0" background="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="test_out4" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="test_out5" type="6" refreshedVersion="0" background="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="test_out5" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="test_out6" type="6" refreshedVersion="0" background="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="test_out6" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="test_out7" type="6" refreshedVersion="0" background="1">
+  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="test_out7" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" name="test_out8" type="6" refreshedVersion="0" background="1">
+  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" name="test_out8" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" name="test_out9" type="6" refreshedVersion="0" background="1">
+  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" name="test_out9" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
@@ -156,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="52">
   <si>
     <t/>
   </si>
@@ -311,6 +314,95 @@
 print("Press Enter to continue...")
 invisible(scan("stdin", character(), nlines = 1, quiet = TRUE))</t>
   </si>
+  <si>
+    <t>testdiagrampython</t>
+  </si>
+  <si>
+    <t>testdiagramperl</t>
+  </si>
+  <si>
+    <t>import matplotlib.pyplot as plt
+import numpy as np
+from inspect import getsourcefile
+from os.path import abspath, dirname
+from os import chdir
+print("changing to script dir..")
+scriptpath = dirname(abspath(getsourcefile(lambda:0)))
+chdir(scriptpath)
+print("loading data ..")
+csvfile = np.loadtxt('test_in.txt',skiprows=1,unpack=True)
+np.savetxt('test_out.txt',csvfile[1])
+print(csvfile[1],csvfile[2])
+print("plotting data ..")
+plt.scatter(csvfile[1],csvfile[2])
+plt.ylabel('in2')
+plt.xlabel('in1')
+plt.savefig("testdiagrampython.png", dpi=300, format='png')
+print("finished ..")</t>
+  </si>
+  <si>
+    <t>use GD::Graph::points;
+open(SRC, '&lt;test_in.txt') or die $!;
+my (@in1, @in2);
+while (&lt;SRC&gt;) {
+    chomp;
+    my @line = split /\t/;
+    next if $line[1] eq "in2";
+    print $line[1]." ... ".$line[2]."\n";
+    push @in1, $line[1];
+    push @in2, $line[2];
+}
+close SRC;
+open(TGT, '&gt;test_out.txt') or die $!;
+print TGT $_."\n" for @in2;
+close TGT;
+print "plotting data\n";
+my @data = ([@in1], [@in2]);
+my $graph = GD::Graph::points-&gt;new(500, 300);
+$graph-&gt;set(
+                        x_label     =&gt; 'in1',
+                        y_label     =&gt; 'in2',
+                    ) or warn $mygraph-&gt;error;
+my $gd = $graph-&gt;plot(\@data) or die $graph-&gt;error;
+open(IMG, '&gt;testdiagramperl.png') or die $!;
+binmode IMG;
+print IMG $gd-&gt;png;
+print "finished \n";</t>
+  </si>
+  <si>
+    <t>var fs, infile;
+var in1 = new Array();
+var arrValues = new Array();
+fs = new ActiveXObject("Scripting.FileSystemObject");
+infile = fs.OpenTextFile("test_in.txt", 1, false);
+var i=0;
+WScript.Echo("reading in file");
+while (infile.AtEndOfStream == false) {
+  line = infile.ReadLine();
+  arrValues = line.split("\t");
+  if (arrValues[1]!="in2") {
+    in1[i]=parseFloat(arrValues[1]);
+    WScript.Echo("in1:"+in1[i]);
+    i++;
+  }
+}
+infile.Close();
+WScript.Echo("writing out file");
+outfile = fs.OpenTextFile("test_out.txt", 2, true);
+for (var i = 0; i &lt; in1.length ; i++) {
+    outfile.WriteLine((in1[i]*2).toString());
+}
+outfile.Close();</t>
+  </si>
+  <si>
+    <t>@echo off
+FOR /F "tokens=2" %%G IN (test_in.txt) DO (
+ IF NOT "%%G" == "in2" (
+      @echo ##### %%G
+      @echo %%G &gt;&gt; test_out.txt
+  )
+)</t>
+  </si>
 </sst>
 </file>
 
@@ -371,74 +463,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -450,7 +480,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -465,20 +495,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -593,16 +628,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1333500</xdr:rowOff>
+      <xdr:rowOff>1362075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -631,7 +666,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7572375" y="161925"/>
+          <a:off x="7896225" y="190500"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -648,23 +683,78 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518172</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>17154</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="testdiagram.png">
+        <xdr:cNvPr id="8" name="testdiagrampython.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286539F7-231E-43AD-BFFA-1550037C67EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CFE719-8492-4496-8EE8-9F51816420E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="0"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>189905</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2695218</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="testdiagramperl.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CDF1B4-27D8-477F-91C5-B70B85A475B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -686,8 +776,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2609850" y="2590800"/>
-          <a:ext cx="4572000" cy="4572000"/>
+          <a:off x="6648450" y="0"/>
+          <a:ext cx="4761905" cy="2857143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -697,6 +787,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Data" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="4" xr16:uid="{D6E1B189-0BFE-45B0-9671-ABBC46A1C935}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1024,12 +1118,12 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O5"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
@@ -1090,7 +1184,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.40250000000000002</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1147,7 +1241,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
-        <v>0.30690000000000001</v>
+        <v>0.50719999999999998</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1204,7 +1298,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
-        <v>1.04E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1260,12 +1354,12 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
-        <v>5.1000000000000004E-3</v>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1321,12 +1415,12 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
-        <v>0.21249999999999999</v>
+        <v>0.28749999999999998</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1356,7 +1450,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
-        <v>5.4999999999999997E-3</v>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1383,14 +1477,14 @@
       <c r="J7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="U7" s="20" t="str">
+      <c r="U7" s="13" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>1.15E-2</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1420,7 +1514,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>1.61E-2</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1450,7 +1544,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
-        <v>2.3E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1480,7 +1574,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
-        <v>0.3836</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1510,7 +1604,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
-        <v>0.34520000000000001</v>
+        <v>0.5706</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1540,7 +1634,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1570,7 +1664,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1600,7 +1694,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
-        <v>1.0200000000000001E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1630,7 +1724,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.40250000000000002</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1660,7 +1754,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.40250000000000002</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1690,7 +1784,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1720,7 +1814,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1750,7 +1844,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>1.61E-2</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1780,7 +1874,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1810,7 +1904,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>1.9099999999999999E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -1840,7 +1934,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
-        <v>4.2500000000000003E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -1870,7 +1964,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>3.8300000000000001E-2</v>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -1900,7 +1994,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
-        <v>0.44500000000000001</v>
+        <v>0.73540000000000005</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -1930,7 +2024,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
-        <v>0.32979999999999998</v>
+        <v>0.54520000000000002</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -1960,7 +2054,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
-        <v>0.36049999999999999</v>
+        <v>0.59589999999999999</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -1990,7 +2084,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
-        <v>0.1918</v>
+        <v>0.317</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -2020,7 +2114,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>1.84E-2</v>
+        <v>3.0499999999999999E-2</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2050,7 +2144,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
-        <v>1.26E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2080,7 +2174,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>1.26E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2110,7 +2204,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2140,7 +2234,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>0.34</v>
+        <v>0.46</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2168,7 +2262,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
-        <v>0.255</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2195,7 +2289,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
-        <v>0.255</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2222,7 +2316,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>0.115</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2249,7 +2343,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
-        <v>1.15E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2276,7 +2370,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
-        <v>6.6E-3</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2303,7 +2397,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
-        <v>6.6E-3</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2330,7 +2424,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
-        <v>2.7000000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2357,7 +2451,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2384,7 +2478,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2411,7 +2505,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
-        <v>1.49E-2</v>
+        <v>2.01E-2</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2438,7 +2532,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>1.15E-2</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2465,7 +2559,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
-        <v>5.9499999999999997E-2</v>
+        <v>8.0500000000000002E-2</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2492,7 +2586,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2519,7 +2613,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
-        <v>3.61E-2</v>
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2546,7 +2640,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2571,10 +2665,13 @@
       </c>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
+        <v>2.3E-2</v>
+      </c>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I50" s="7"/>
     </row>
   </sheetData>
@@ -2592,8 +2689,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2686,7 +2783,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210710/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210728/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2720,7 +2817,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20210710/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20210728/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2812,7 +2909,7 @@
       </c>
       <c r="C18" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -2829,7 +2926,7 @@
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210710</v>
+        <v>unterverz/unterunterverz/20210728</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -2848,10 +2945,10 @@
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C21"/>
@@ -2862,10 +2959,10 @@
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C22"/>
@@ -2875,24 +2972,24 @@
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C23"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="14"/>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C24"/>
@@ -2903,7 +3000,7 @@
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -2918,7 +3015,7 @@
     </row>
     <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26"/>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C26"/>
@@ -9014,7 +9111,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="eingabeToy"/>
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J7" sqref="J7:L12"/>
@@ -9065,12 +9162,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="12">
         <v>0.5</v>
       </c>
       <c r="D2">
@@ -9098,12 +9195,12 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="12">
         <v>0.6</v>
       </c>
       <c r="D3">
@@ -9132,12 +9229,12 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="12">
         <v>0.8</v>
       </c>
       <c r="D4">
@@ -9164,7 +9261,9 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5"/>
+      <c r="A5">
+        <v>0</v>
+      </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
@@ -9173,10 +9272,14 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6"/>
+      <c r="A6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7"/>
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="J7" s="4" t="s">
         <v>18</v>
       </c>
@@ -9187,10 +9290,12 @@
         <v>40</v>
       </c>
       <c r="O7" s="4"/>
-      <c r="P7" s="23"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8"/>
+      <c r="A8">
+        <v>0</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="J8" s="4" t="s">
         <v>2</v>
@@ -9202,7 +9307,9 @@
       <c r="P8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9"/>
+      <c r="A9">
+        <v>0</v>
+      </c>
       <c r="J9" s="3" t="s">
         <v>1</v>
       </c>
@@ -9213,7 +9320,9 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10"/>
+      <c r="A10">
+        <v>0</v>
+      </c>
       <c r="J10" s="3" t="s">
         <v>6</v>
       </c>
@@ -9224,7 +9333,9 @@
       <c r="P10"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11"/>
+      <c r="A11">
+        <v>0</v>
+      </c>
       <c r="J11" s="3" t="s">
         <v>5</v>
       </c>
@@ -9235,7 +9346,9 @@
       <c r="P11"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12"/>
+      <c r="A12">
+        <v>0</v>
+      </c>
       <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
@@ -9246,110 +9359,185 @@
       <c r="P12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13"/>
+      <c r="A13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14"/>
+      <c r="A14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15"/>
+      <c r="A15">
+        <v>0</v>
+      </c>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16"/>
+      <c r="A16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17"/>
+      <c r="A17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18"/>
+      <c r="A18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19"/>
+      <c r="A19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20"/>
+      <c r="A20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21"/>
+      <c r="A21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22"/>
+      <c r="A22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23"/>
+      <c r="A23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24"/>
+      <c r="A24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25"/>
+      <c r="A25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26"/>
+      <c r="A26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27"/>
+      <c r="A27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28"/>
+      <c r="A28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29"/>
+      <c r="A29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30"/>
+      <c r="A30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31"/>
+      <c r="A31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32"/>
+      <c r="A32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33"/>
+      <c r="A33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34"/>
+      <c r="A34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35"/>
+      <c r="A35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36"/>
+      <c r="A36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37"/>
+      <c r="A37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38"/>
+      <c r="A38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39"/>
+      <c r="A39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40"/>
+      <c r="A40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41"/>
+      <c r="A41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42"/>
+      <c r="A42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43"/>
+      <c r="A43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44"/>
+      <c r="A44">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45"/>
+      <c r="A45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46"/>
+      <c r="A46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47"/>
+      <c r="A47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -9357,6 +9545,227 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E53A6E-2604-4578-8654-8C7F2E62C0EC}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65D33DA-8813-4379-A28B-0EF367670337}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="344.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D836FE-DB83-4BD9-ADBD-5E2BC66117E2}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="48.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="293.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CF1B26-A656-4BDC-B33A-EB9111C2BAE8}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="83.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added executeScript (from VBA) fixed problems in testScriptAddin.xlsx added skipscript type added SkipPreparationAndExec (Ctrl Key) added doc for settings and new features
</commit_message>
<xml_diff>
--- a/test/testScriptAddin.xlsx
+++ b/test/testScriptAddin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ScriptAddin\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB98C77-AA4F-4998-BC95-F8691647DA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB85DC-431E-468C-83EB-DB804DFE381D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="765" windowWidth="23790" windowHeight="14925" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -22,30 +22,30 @@
     <sheet name="Test_cmdshell" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="Data" localSheetId="2">Test_OtherSheet!$A$2:$A$48</definedName>
-    <definedName name="Script_" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
-    <definedName name="Script_">'Main Test'!$J$1:$L$5</definedName>
-    <definedName name="Script_AnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
-    <definedName name="Script_AnotherDef">'Main Test'!$M$1:$O$5</definedName>
-    <definedName name="Script_ErrorInDef">'Main Test'!$P$1:$R$5</definedName>
-    <definedName name="Script_NewResDiagDir">'Main Test'!$S$1:$U$5</definedName>
-    <definedName name="Script_ScriptCell" localSheetId="1">Test_scriptRng!$A$21:$C$25</definedName>
-    <definedName name="Script_ScriptRange" localSheetId="1">Test_scriptRng!$A$15:$C$19</definedName>
-    <definedName name="Script_TestCmdShell">Test_cmdshell!$A$1:$C$4</definedName>
-    <definedName name="Script_TestJscriptCell">Test_cscript!$A$1:$C$4</definedName>
-    <definedName name="Script_TestPerlCell">Test_perl!$A$1:$C$5</definedName>
-    <definedName name="Script_TestPythonCell">Test_python!$A$1:$C$5</definedName>
+    <definedName name="Script_" localSheetId="2">Test_OtherSheet!$J$1:$L$6</definedName>
+    <definedName name="Script_">'Main Test'!$J$1:$L$6</definedName>
+    <definedName name="Script_AnotherDef" localSheetId="2">Test_OtherSheet!$J$8:$L$14</definedName>
+    <definedName name="Script_AnotherDef">'Main Test'!$M$1:$O$6</definedName>
+    <definedName name="Script_Choice">'Main Test'!$Q$13:$S$19</definedName>
+    <definedName name="Script_ErrorInDef">'Main Test'!$P$1:$R$6</definedName>
+    <definedName name="Script_NewResDiagDir">'Main Test'!$S$1:$U$6</definedName>
+    <definedName name="Script_ScriptCell" localSheetId="1">Test_scriptRng!$A$22:$C$27</definedName>
+    <definedName name="Script_ScriptRange" localSheetId="1">Test_scriptRng!$A$15:$C$20</definedName>
+    <definedName name="Script_TestCmdShell">Test_cmdshell!$A$1:$C$5</definedName>
+    <definedName name="Script_TestCscriptCell">Test_cscript!$A$1:$C$5</definedName>
+    <definedName name="Script_TestPerlCell">Test_perl!$A$1:$C$6</definedName>
+    <definedName name="Script_TestPythonCell">Test_python!$A$1:$C$6</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$13</definedName>
     <definedName name="test_in" localSheetId="2">Test_OtherSheet!$B$1:$H$4</definedName>
     <definedName name="test_in">'Main Test'!$B$1:$H$301</definedName>
     <definedName name="test_out" localSheetId="2">Test_OtherSheet!$A$2:$A$4</definedName>
     <definedName name="test_out">'Main Test'!$A$2:$A$49</definedName>
-    <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$17</definedName>
+    <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$19</definedName>
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
-    <definedName name="testdiagram">'Main Test'!$J$8</definedName>
+    <definedName name="testdiagram">'Main Test'!$J$9</definedName>
     <definedName name="testdiagramperl">Test_perl!$E$1</definedName>
     <definedName name="testdiagrampython">Test_python!$D$1</definedName>
-    <definedName name="variablesVerzeichnis">'Main Test'!$U$7</definedName>
+    <definedName name="variablesVerzeichnis">'Main Test'!$U$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,104 +62,32 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="test_out" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="test_out1" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="test_out10" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="4" xr16:uid="{410C0FA3-7542-41AB-90A9-C19D5D697CAD}" name="test_out11" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr prompt="0" sourceFile="C:\dev\ScriptAddin\test\.\test_out.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="test_out2" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="test_out21" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out2.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="test_out3" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="test_out4" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="test_out5" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="test_out6" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="test_out7" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" name="test_out8" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" name="test_out9" type="6" refreshedVersion="0" background="1">
-    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>roland kapl</author>
+  </authors>
+  <commentList>
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{399BBC05-A1C3-4CA2-9DB5-178DFE30B290}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>actually this doesn't matter here, as it is overruled by exec/rexec
+Just need it for avoiding stderr msgs preventing returning the result</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="60">
   <si>
     <t/>
   </si>
@@ -270,9 +198,6 @@
   </si>
   <si>
     <t>scriptCell</t>
-  </si>
-  <si>
-    <t>argc</t>
   </si>
   <si>
     <t>-&gt; Attention, diagram for test_scriptcell appears in Main Test !!!</t>
@@ -403,6 +328,47 @@
   )
 )</t>
   </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>library(ggplot2)
+initial.options &lt;- commandArgs(trailingOnly = FALSE)
+script.name &lt;- sub("--file=", "", initial.options[grep("--file=", initial.options)])
+script.basename &lt;- dirname(script.name)
+if (length(script.basename) &gt; 0) {
+   setwd(script.basename)
+   test_in &lt;- read.csv2("test_in.txt",dec=".",sep="\t",header=TRUE)
+   write.table(test_in[,1],file="test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)
+}
+test_out&lt;-test_in[,1]
+print(getwd())
+gplot &lt;- ggplot(data = test_in, aes(x = in3, y = in4) ) + geom_point()
+png(filename="testdiagram.png")
+print(gplot)
+dev.off()</t>
+  </si>
+  <si>
+    <t>choose to run:</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Perl</t>
+  </si>
+  <si>
+    <t>Cscript</t>
+  </si>
+  <si>
+    <t>WinCmd</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
 </sst>
 </file>
 
@@ -414,7 +380,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -448,8 +414,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,8 +447,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -471,16 +461,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -514,8 +520,13 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="6" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Eingabe" xfId="6" builtinId="20"/>
     <cellStyle name="Komma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Prozent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -575,21 +586,21 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="testdiagram.png">
+        <xdr:cNvPr id="7" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24127001-D2AE-44EC-B8F6-7705BFD4AF16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B94FE94-97BC-4C15-8AFB-2454F504DEF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -611,7 +622,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828925" y="1133475"/>
+          <a:off x="2819400" y="1295400"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -628,23 +639,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>1362075</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1009650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagram.png">
+        <xdr:cNvPr id="6" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{741ECA18-5151-42F1-AB02-52E961ECE795}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{682F7A07-2B5F-4757-BFD7-D3067F737ADB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -666,7 +677,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7896225" y="190500"/>
+          <a:off x="7572375" y="161925"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -683,6 +694,61 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="testdiagram.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D999D498-28F5-4F82-AD66-D6B31ACB898C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2609850" y="2914650"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -696,10 +762,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="testdiagrampython.png">
+        <xdr:cNvPr id="3" name="testdiagrampython.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CFE719-8492-4496-8EE8-9F51816420E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E85460C-52BD-45E1-BCA5-19EE7C3581EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -734,7 +800,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -746,15 +812,15 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>189905</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2695218</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2533293</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="testdiagramperl.png">
+        <xdr:cNvPr id="4" name="testdiagramperl.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CDF1B4-27D8-477F-91C5-B70B85A475B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD19027B-10EC-41B6-B2F1-3B8D3046D759}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -787,10 +853,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Data" growShrinkType="overwriteClear" adjustColumnWidth="0" connectionId="4" xr16:uid="{D6E1B189-0BFE-45B0-9671-ABBC46A1C935}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1117,8 +1179,8 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1129,7 +1191,8 @@
     <col min="6" max="7" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -1178,13 +1241,13 @@
         <v>2</v>
       </c>
       <c r="T1" t="str">
-        <f ca="1">SUBSTITUTE(CELL("DATEINAME",U1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\ScriptAddin\test\[testScriptAddin.xlsx]Main Test</v>
+        <f ca="1">SUBSTITUTE(CELL("DATEINAME",U1),"[testScriptAddin.xlsx]Main Test","")</f>
+        <v>C:\dev\ScriptAddin\test\</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
-        <v>0.40250000000000002</v>
+        <v>0.29749999999999999</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1208,40 +1271,34 @@
         <v>-1.8899999999999995</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>35</v>
+      <c r="J2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
-        <v>0.50719999999999998</v>
+        <v>0.30690000000000001</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1266,39 +1323,39 @@
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="R3" t="s">
         <v>34</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
-        <v>1.7100000000000001E-2</v>
+        <v>1.04E-2</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1323,43 +1380,39 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O4" t="s">
         <v>33</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R4" t="s">
         <v>34</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T4" t="s">
-        <v>10</v>
-      </c>
-      <c r="U4" t="str">
-        <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210728</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
-        <v>6.8999999999999999E-3</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1384,43 +1437,43 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O5" t="s">
         <v>33</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="R5" t="s">
         <v>34</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210728</v>
+        <v>unterverz/unterunterverz/20210730</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
-        <v>0.28749999999999998</v>
+        <v>0.21249999999999999</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1444,13 +1497,45 @@
         <v>-1.35</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
       <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="M6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" t="str">
+        <f ca="1">variablesVerzeichnis</f>
+        <v>unterverz/unterunterverz/20210730</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
-        <v>8.8999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1477,14 +1562,10 @@
       <c r="J7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="U7" s="13" t="str">
-        <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20210728</v>
-      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
-        <v>1.15E-2</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1511,10 +1592,14 @@
       <c r="J8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
+      <c r="U8" s="13" t="str">
+        <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
+        <v>unterverz/unterunterverz/20210730</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
-        <v>1.61E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1544,7 +1629,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
-        <v>3.1099999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1574,7 +1659,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
-        <v>0.63400000000000001</v>
+        <v>0.3836</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1601,10 +1686,16 @@
       <c r="J11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
+      <c r="Q11" t="s">
+        <v>54</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
-        <v>0.5706</v>
+        <v>0.34520000000000001</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1634,7 +1725,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
-        <v>2.4E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1661,10 +1752,16 @@
       <c r="J13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
+      <c r="Q13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
-        <v>2.4E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1691,10 +1788,16 @@
       <c r="J14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
+      <c r="Q14" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="R14" s="26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
-        <v>1.38E-2</v>
+        <v>1.0200000000000001E-2</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1721,10 +1824,17 @@
       <c r="J15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
+      <c r="Q15" s="3" t="str">
+        <f>IF($R$11="testScript.R","script","skipscript")</f>
+        <v>script</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>0.40250000000000002</v>
+        <v>0.29749999999999999</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1751,10 +1861,17 @@
       <c r="J16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q16" s="3" t="str">
+        <f>IF($R$11="testScript.R","skipscript","scriptCell")</f>
+        <v>skipscript</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>0.40250000000000002</v>
+        <v>0.29749999999999999</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1781,10 +1898,16 @@
       <c r="J17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1811,10 +1934,16 @@
       <c r="J18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1841,10 +1970,16 @@
       <c r="J19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>1.61E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1872,9 +2007,9 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>2.3E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1902,9 +2037,9 @@
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>2.5899999999999999E-2</v>
+        <v>1.9099999999999999E-2</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -1932,9 +2067,9 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
-        <v>5.7500000000000002E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -1962,9 +2097,9 @@
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>5.1799999999999999E-2</v>
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -1992,9 +2127,9 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
-        <v>0.73540000000000005</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -2022,9 +2157,9 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
-        <v>0.54520000000000002</v>
+        <v>0.32979999999999998</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -2052,9 +2187,9 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
-        <v>0.59589999999999999</v>
+        <v>0.36049999999999999</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -2082,9 +2217,9 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
-        <v>0.317</v>
+        <v>0.1918</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -2112,9 +2247,9 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>3.0499999999999999E-2</v>
+        <v>1.84E-2</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2142,9 +2277,9 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
-        <v>2.0899999999999998E-2</v>
+        <v>1.26E-2</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2172,9 +2307,9 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>2.0899999999999998E-2</v>
+        <v>1.26E-2</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2202,9 +2337,9 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2232,9 +2367,9 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>0.46</v>
+        <v>0.34</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2259,10 +2394,11 @@
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M33" s="7"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
-        <v>0.34499999999999997</v>
+        <v>0.255</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2286,10 +2422,11 @@
         <v>-1.62</v>
       </c>
       <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
-        <v>0.34499999999999997</v>
+        <v>0.255</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2314,9 +2451,9 @@
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
-        <v>0.115</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2341,9 +2478,9 @@
       </c>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
-        <v>1.9E-2</v>
+        <v>1.15E-2</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2368,9 +2505,9 @@
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
-        <v>1.0800000000000001E-2</v>
+        <v>6.6E-3</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2395,9 +2532,9 @@
       </c>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
-        <v>1.0800000000000001E-2</v>
+        <v>6.6E-3</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2422,9 +2559,9 @@
       </c>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
-        <v>4.4000000000000003E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2449,9 +2586,9 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
-        <v>4.5999999999999999E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2476,9 +2613,9 @@
       </c>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
-        <v>2.3E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2503,9 +2640,9 @@
       </c>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
-        <v>2.01E-2</v>
+        <v>1.49E-2</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2530,9 +2667,9 @@
       </c>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
-        <v>1.15E-2</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2557,9 +2694,9 @@
       </c>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
-        <v>8.0500000000000002E-2</v>
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2584,9 +2721,9 @@
       </c>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
-        <v>4.5999999999999999E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2611,9 +2748,9 @@
       </c>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
-        <v>4.8899999999999999E-2</v>
+        <v>3.61E-2</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2638,9 +2775,9 @@
       </c>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
-        <v>2.3E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2675,6 +2812,11 @@
       <c r="I50" s="7"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R11" xr:uid="{D48B4262-C350-4C0A-9421-E16722C32D68}">
+      <formula1>"testScript.R,script in cell"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -2687,17 +2829,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:M298"/>
+  <dimension ref="A1:M300"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A22" sqref="A22:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="11" customWidth="1"/>
     <col min="2" max="2" width="94.5703125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="11" customWidth="1"/>
     <col min="4" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
     <col min="18" max="18" width="86.5703125" customWidth="1"/>
@@ -2749,7 +2891,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2760,7 +2902,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2771,7 +2913,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2783,7 +2925,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210728/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210730/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2805,7 +2947,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2817,7 +2959,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20210728/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20210730/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2873,11 +3015,11 @@
       <c r="H15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>35</v>
+      <c r="A16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -2888,10 +3030,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -2902,15 +3044,12 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="str">
-        <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210728</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -2919,14 +3058,14 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210728</v>
+        <v>unterverz/unterunterverz/20210730</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -2935,9 +3074,16 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="str">
+        <f ca="1">variablesVerzeichnis</f>
+        <v>unterverz/unterunterverz/20210730</v>
+      </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -2945,12 +3091,8 @@
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>3</v>
-      </c>
+      <c r="A21"/>
+      <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
@@ -2958,12 +3100,12 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>45</v>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>3</v>
       </c>
       <c r="C22"/>
       <c r="E22"/>
@@ -2972,11 +3114,11 @@
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>9</v>
+      <c r="A23" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="C23"/>
       <c r="D23" s="14"/>
@@ -2985,12 +3127,12 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -3001,10 +3143,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -3013,10 +3155,12 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A26"/>
-      <c r="B26" s="15" t="s">
-        <v>38</v>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -3026,8 +3170,12 @@
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27"/>
-      <c r="B27"/>
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
@@ -3035,9 +3183,11 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A28"/>
-      <c r="B28"/>
+      <c r="B28" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
@@ -3186,12 +3336,9 @@
       <c r="H42"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>0</v>
-      </c>
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
       <c r="D43" s="11" t="s">
         <v>0</v>
       </c>
@@ -3212,12 +3359,9 @@
       <c r="M43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B44" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>0</v>
-      </c>
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
       <c r="D44" s="11" t="s">
         <v>0</v>
       </c>
@@ -9095,6 +9239,22 @@
         <v>0</v>
       </c>
       <c r="H298" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B299" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C299" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B300" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C300" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9109,12 +9269,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="eingabeToy"/>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L12"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9162,7 +9322,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -9186,16 +9346,17 @@
         <v>3</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="J2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -9221,15 +9382,15 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -9254,290 +9415,214 @@
         <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="J5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6"/>
+      <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>0</v>
-      </c>
-    </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7"/>
       <c r="O7" s="4"/>
       <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>0</v>
-      </c>
+      <c r="A8"/>
       <c r="C8" s="6"/>
       <c r="J8" s="4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>3</v>
+        <v>38</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>19</v>
+      <c r="A9"/>
+      <c r="J9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>6</v>
+      <c r="A10"/>
+      <c r="J10" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0</v>
-      </c>
+      <c r="A11"/>
       <c r="J11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>0</v>
-      </c>
+      <c r="A12"/>
       <c r="J12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>0</v>
+      <c r="A13"/>
+      <c r="J13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0</v>
+      <c r="A14"/>
+      <c r="J14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>0</v>
-      </c>
+      <c r="A15"/>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>0</v>
-      </c>
+      <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0</v>
-      </c>
+      <c r="A17"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0</v>
-      </c>
+      <c r="A18"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0</v>
-      </c>
+      <c r="A19"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>0</v>
-      </c>
+      <c r="A20"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>0</v>
-      </c>
+      <c r="A21"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>0</v>
-      </c>
+      <c r="A22"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0</v>
-      </c>
+      <c r="A23"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>0</v>
-      </c>
+      <c r="A24"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>0</v>
-      </c>
+      <c r="A25"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>0</v>
-      </c>
+      <c r="A26"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>0</v>
-      </c>
+      <c r="A27"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>0</v>
-      </c>
+      <c r="A28"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>0</v>
-      </c>
+      <c r="A29"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>0</v>
-      </c>
+      <c r="A30"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>0</v>
-      </c>
+      <c r="A31"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>0</v>
-      </c>
+      <c r="A32"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>0</v>
-      </c>
+      <c r="A33"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>0</v>
-      </c>
+      <c r="A34"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>0</v>
-      </c>
+      <c r="A35"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>0</v>
-      </c>
+      <c r="A36"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>0</v>
-      </c>
+      <c r="A37"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>0</v>
-      </c>
+      <c r="A38"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>0</v>
-      </c>
+      <c r="A39"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>0</v>
-      </c>
+      <c r="A40"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>0</v>
-      </c>
+      <c r="A41"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>0</v>
-      </c>
+      <c r="A42"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>0</v>
-      </c>
+      <c r="A43"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>0</v>
-      </c>
+      <c r="A44"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>0</v>
-      </c>
+      <c r="A45"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>0</v>
-      </c>
+      <c r="A46"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
-        <v>0</v>
-      </c>
+      <c r="A47"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -9545,15 +9630,17 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E53A6E-2604-4578-8654-8C7F2E62C0EC}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9569,36 +9656,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="242.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>9</v>
+      <c r="B3" s="19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>46</v>
+      <c r="B6" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -9609,10 +9704,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65D33DA-8813-4379-A28B-0EF367670337}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9628,40 +9723,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="344.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="344.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>9</v>
+      <c r="B3" s="19" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="20"/>
+      <c r="B6" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9671,10 +9774,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D836FE-DB83-4BD9-ADBD-5E2BC66117E2}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9690,27 +9793,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="293.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="293.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>9</v>
+      <c r="B3" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9722,10 +9833,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CF1B26-A656-4BDC-B33A-EB9111C2BAE8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9741,27 +9852,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>9</v>
+      <c r="B3" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bug with std input (still has problems with backspace) fixed bug with closing out window with Esc added example insertion added possibility to pass arguments to scripts added possibility to have other extensions than .txt for arg and result files
</commit_message>
<xml_diff>
--- a/test/testScriptAddin.xlsx
+++ b/test/testScriptAddin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ScriptAddin\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB85DC-431E-468C-83EB-DB804DFE381D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C7128-2494-47E7-9D10-55DA543EAD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="570" windowWidth="23760" windowHeight="13425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -266,35 +266,6 @@
 print("finished ..")</t>
   </si>
   <si>
-    <t>use GD::Graph::points;
-open(SRC, '&lt;test_in.txt') or die $!;
-my (@in1, @in2);
-while (&lt;SRC&gt;) {
-    chomp;
-    my @line = split /\t/;
-    next if $line[1] eq "in2";
-    print $line[1]." ... ".$line[2]."\n";
-    push @in1, $line[1];
-    push @in2, $line[2];
-}
-close SRC;
-open(TGT, '&gt;test_out.txt') or die $!;
-print TGT $_."\n" for @in2;
-close TGT;
-print "plotting data\n";
-my @data = ([@in1], [@in2]);
-my $graph = GD::Graph::points-&gt;new(500, 300);
-$graph-&gt;set(
-                        x_label     =&gt; 'in1',
-                        y_label     =&gt; 'in2',
-                    ) or warn $mygraph-&gt;error;
-my $gd = $graph-&gt;plot(\@data) or die $graph-&gt;error;
-open(IMG, '&gt;testdiagramperl.png') or die $!;
-binmode IMG;
-print IMG $gd-&gt;png;
-print "finished \n";</t>
-  </si>
-  <si>
     <t>var fs, infile;
 var in1 = new Array();
 var arrValues = new Array();
@@ -368,6 +339,39 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>use GD::Graph::points;
+open(SRC, '&lt;test_in.txt') or die $!;
+my (@in1, @in2);
+$|=1;
+print "enter some value:\n";
+my $val = &lt;&gt;;
+print "value: $val\n";
+while (&lt;SRC&gt;) {
+    chomp;
+    my @line = split /\t/;
+    next if $line[1] eq "in2";
+    print $line[1]." ... ".$line[2]."\n";
+    push @in1, $line[1];
+    push @in2, $line[2];
+}
+close SRC;
+open(TGT, '&gt;test_out.txt') or die $!;
+print TGT $_."\n" for @in2;
+close TGT;
+print "plotting data\n";
+my @data = ([@in1], [@in2]);
+my $graph = GD::Graph::points-&gt;new(500, 300);
+$graph-&gt;set(
+                        x_label     =&gt; 'in1',
+                        y_label     =&gt; 'in2',
+                    ) or warn $mygraph-&gt;error;
+my $gd = $graph-&gt;plot(\@data) or die $graph-&gt;error;
+open(IMG, '&gt;testdiagramperl.png') or die $!;
+binmode IMG;
+print IMG $gd-&gt;png;
+print "finished \n";</t>
   </si>
 </sst>
 </file>
@@ -817,10 +821,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagramperl.png">
+        <xdr:cNvPr id="28" name="testdiagramperl.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD19027B-10EC-41B6-B2F1-3B8D3046D759}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C7D6EF7-96F3-4146-921C-ECCA8FDB7D52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1179,7 +1183,7 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -1247,7 +1251,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1272,33 +1276,33 @@
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="M2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="P2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="S2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
-        <v>0.30690000000000001</v>
+        <v>0.81410000000000005</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1355,7 +1359,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
-        <v>1.04E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1412,7 +1416,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
-        <v>5.1000000000000004E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1468,12 +1472,12 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210730</v>
+        <v>unterverz/unterunterverz/20211222</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
-        <v>0.21249999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1530,12 +1534,12 @@
       </c>
       <c r="U6" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210730</v>
+        <v>unterverz/unterunterverz/20211222</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
-        <v>5.4999999999999997E-3</v>
+        <v>1.44E-2</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1565,7 +1569,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1594,12 +1598,12 @@
       <c r="M8" s="7"/>
       <c r="U8" s="13" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20210730</v>
+        <v>unterverz/unterunterverz/20211222</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1629,7 +1633,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
-        <v>2.3E-2</v>
+        <v>5.4100000000000002E-2</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1659,7 +1663,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
-        <v>0.3836</v>
+        <v>1.0176000000000001</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1687,7 +1691,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="Q11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R11" s="24" t="s">
         <v>8</v>
@@ -1695,7 +1699,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
-        <v>0.34520000000000001</v>
+        <v>0.91579999999999995</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1725,7 +1729,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1761,7 +1765,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1789,15 +1793,15 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="Q14" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="R14" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="R14" s="26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
-        <v>1.0200000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1834,7 +1838,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1866,12 +1870,12 @@
         <v>skipscript</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1907,7 +1911,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1943,7 +1947,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1979,7 +1983,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -2009,7 +2013,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2039,7 +2043,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>1.9099999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -2069,7 +2073,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
-        <v>4.2500000000000003E-2</v>
+        <v>0.1</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -2099,7 +2103,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>3.8300000000000001E-2</v>
+        <v>9.01E-2</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -2129,7 +2133,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
-        <v>0.44500000000000001</v>
+        <v>1.1803999999999999</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -2159,7 +2163,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
-        <v>0.32979999999999998</v>
+        <v>0.875</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -2189,7 +2193,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
-        <v>0.36049999999999999</v>
+        <v>0.95640000000000003</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -2219,7 +2223,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
-        <v>0.1918</v>
+        <v>0.50880000000000003</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -2249,7 +2253,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>1.84E-2</v>
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2279,7 +2283,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
-        <v>1.26E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2309,7 +2313,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>1.26E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2339,7 +2343,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2369,7 +2373,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>0.34</v>
+        <v>0.8</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2398,7 +2402,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
-        <v>0.255</v>
+        <v>0.6</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2426,7 +2430,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
-        <v>0.255</v>
+        <v>0.6</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2453,7 +2457,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>0.2</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2480,7 +2484,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
-        <v>1.15E-2</v>
+        <v>3.0499999999999999E-2</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2507,7 +2511,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
-        <v>6.6E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2534,7 +2538,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
-        <v>6.6E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2561,7 +2565,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
-        <v>2.7000000000000001E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2588,7 +2592,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2615,7 +2619,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2642,7 +2646,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
-        <v>1.49E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2669,7 +2673,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2696,7 +2700,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
-        <v>5.9499999999999997E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2723,7 +2727,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2750,7 +2754,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
-        <v>3.61E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2777,7 +2781,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2831,7 +2835,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M300"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:C27"/>
     </sheetView>
   </sheetViews>
@@ -2925,7 +2929,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210730/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20211222/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2959,7 +2963,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20210730/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20211222/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -3016,10 +3020,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>52</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -3065,7 +3069,7 @@
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210730</v>
+        <v>unterverz/unterunterverz/20211222</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -3082,7 +3086,7 @@
       </c>
       <c r="C20" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210730</v>
+        <v>unterverz/unterunterverz/20211222</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
@@ -3115,10 +3119,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>52</v>
       </c>
       <c r="C23"/>
       <c r="D23" s="14"/>
@@ -9347,10 +9351,10 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>52</v>
       </c>
       <c r="L2"/>
     </row>
@@ -9462,13 +9466,13 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="J9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="2"/>
@@ -9658,10 +9662,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="242.25" x14ac:dyDescent="0.2">
@@ -9706,8 +9710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65D33DA-8813-4379-A28B-0EF367670337}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9725,18 +9729,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="344.25" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="395.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -9795,10 +9799,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="293.25" x14ac:dyDescent="0.2">
@@ -9806,7 +9810,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -9854,10 +9858,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
@@ -9865,7 +9869,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>